<commit_message>
starting the remade procedure for figure 1
</commit_message>
<xml_diff>
--- a/Data/sgRNA/Figure6/impurity.xlsx
+++ b/Data/sgRNA/Figure6/impurity.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15000"/>
+    <workbookView windowHeight="14980"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="13">
   <si>
     <t>base_name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>5+23</t>
   </si>
   <si>
     <t>ladder24</t>
@@ -1244,13 +1247,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G178"/>
+  <dimension ref="A1:H178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108:G116"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="11.125" customWidth="1"/>
     <col min="2" max="2" width="19.0625" customWidth="1"/>
@@ -1258,6 +1261,7 @@
     <col min="4" max="4" width="12.6875" customWidth="1"/>
     <col min="5" max="5" width="10.4375" customWidth="1"/>
     <col min="6" max="6" width="14.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6875"/>
     <col min="10" max="10" width="12.6875"/>
     <col min="11" max="11" width="10.5"/>
     <col min="12" max="12" width="12.6875"/>
@@ -1289,7 +1293,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="2:7">
+    <row r="2" spans="2:8">
       <c r="B2" s="2">
         <v>6467.80156240349</v>
       </c>
@@ -1308,6 +1312,10 @@
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <f>B2/320</f>
+        <v>20.2118798825109</v>
+      </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="2" t="s">
@@ -1549,7 +1557,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:8">
       <c r="A13" s="2"/>
       <c r="B13" s="2">
         <v>6757.90107404547</v>
@@ -1570,6 +1578,10 @@
       <c r="G13">
         <v>1</v>
       </c>
+      <c r="H13">
+        <f>B13/320</f>
+        <v>21.1184408563921</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" s="2" t="s">
@@ -2119,7 +2131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="2:7">
+    <row r="37" spans="2:8">
       <c r="B37" s="2">
         <v>1293.18464636066</v>
       </c>
@@ -2137,6 +2149,10 @@
       </c>
       <c r="G37">
         <v>1</v>
+      </c>
+      <c r="H37">
+        <f>B37/320</f>
+        <v>4.04120201987706</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -2547,7 +2563,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="2:7">
+    <row r="55" spans="2:8">
       <c r="B55" s="2">
         <v>1959.26824760388</v>
       </c>
@@ -2567,6 +2583,10 @@
       <c r="G55">
         <v>1</v>
       </c>
+      <c r="H55">
+        <f>B55/320</f>
+        <v>6.12271327376213</v>
+      </c>
     </row>
     <row r="56" spans="1:7">
       <c r="A56" s="2" t="s">
@@ -3237,7 +3257,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="84" spans="2:7">
+    <row r="84" spans="2:8">
       <c r="B84" s="2">
         <v>9705.29948843839</v>
       </c>
@@ -3257,6 +3277,10 @@
       <c r="G84">
         <v>1</v>
       </c>
+      <c r="H84">
+        <f>B84/320</f>
+        <v>30.32906090137</v>
+      </c>
     </row>
     <row r="85" spans="1:7">
       <c r="A85" s="2" t="s">
@@ -3546,7 +3570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="97" spans="2:7">
+    <row r="97" spans="2:8">
       <c r="B97" s="2">
         <v>3270.46172823274</v>
       </c>
@@ -3566,6 +3590,10 @@
       <c r="G97">
         <v>1</v>
       </c>
+      <c r="H97">
+        <f>B97/320</f>
+        <v>10.2201929007273</v>
+      </c>
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="2" t="s">
@@ -3807,7 +3835,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="108" spans="2:7">
+    <row r="108" spans="2:8">
       <c r="B108" s="2">
         <v>3184.40652842222</v>
       </c>
@@ -3827,6 +3855,10 @@
       <c r="G108" s="5">
         <v>1</v>
       </c>
+      <c r="H108">
+        <f>B108/320</f>
+        <v>9.95127040131944</v>
+      </c>
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="2" t="s">
@@ -3869,7 +3901,7 @@
         <v>33</v>
       </c>
       <c r="F110" s="2">
-        <f t="shared" ref="F110:F115" si="8">F109</f>
+        <f t="shared" ref="F110:F116" si="8">F109</f>
         <v>23</v>
       </c>
       <c r="G110" s="5">
@@ -4013,14 +4045,14 @@
         <v>33</v>
       </c>
       <c r="F116" s="2">
-        <f>F115</f>
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="G116" s="5">
         <v>9</v>
       </c>
     </row>
-    <row r="117" spans="1:7">
+    <row r="117" spans="1:8">
       <c r="A117" s="2"/>
       <c r="B117" s="2">
         <v>1622.23735218323</v>
@@ -4040,6 +4072,10 @@
       <c r="G117">
         <v>1</v>
       </c>
+      <c r="H117">
+        <f>B117/320</f>
+        <v>5.06949172557259</v>
+      </c>
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="2" t="s">
@@ -4082,7 +4118,7 @@
         <v>35</v>
       </c>
       <c r="F119" s="2">
-        <f t="shared" ref="F119:F139" si="9">F118</f>
+        <f t="shared" ref="F119:F140" si="9">F118</f>
         <v>25</v>
       </c>
       <c r="G119">
@@ -4569,7 +4605,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="140" spans="1:7">
+    <row r="140" spans="1:8">
       <c r="A140" s="2" t="s">
         <v>9</v>
       </c>
@@ -4586,14 +4622,17 @@
         <v>35</v>
       </c>
       <c r="F140" s="2">
-        <f>F139</f>
+        <f t="shared" si="9"/>
         <v>25</v>
       </c>
       <c r="G140">
         <v>24</v>
       </c>
-    </row>
-    <row r="141" spans="2:7">
+      <c r="H140" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="141" spans="2:8">
       <c r="B141" s="2">
         <v>1920.24499025174</v>
       </c>
@@ -4613,6 +4652,10 @@
       <c r="G141">
         <v>1</v>
       </c>
+      <c r="H141">
+        <f>B141/320</f>
+        <v>6.00076559453669</v>
+      </c>
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="2" t="s">
@@ -5152,7 +5195,7 @@
         <v>34</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G164" s="5">
         <v>1</v>
@@ -5175,7 +5218,7 @@
         <v>34</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G165" s="5">
         <v>2</v>
@@ -5198,7 +5241,7 @@
         <v>34</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G166" s="5">
         <v>3</v>
@@ -5221,7 +5264,7 @@
         <v>34</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G167" s="5">
         <v>4</v>
@@ -5244,7 +5287,7 @@
         <v>34</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G168" s="5">
         <v>5</v>
@@ -5267,7 +5310,7 @@
         <v>34</v>
       </c>
       <c r="F169" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G169" s="5">
         <v>6</v>
@@ -5290,7 +5333,7 @@
         <v>34</v>
       </c>
       <c r="F170" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G170" s="5">
         <v>7</v>

</xml_diff>